<commit_message>
inseridas opções de radion button das unidades
</commit_message>
<xml_diff>
--- a/arquivos/IW_PROD_RJ_Lista.xlsx
+++ b/arquivos/IW_PROD_RJ_Lista.xlsx
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,485 +403,496 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2">
-        <v>45349</v>
+        <v>45380</v>
       </c>
       <c r="C2" s="2">
-        <v>45379</v>
+        <v>45409</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
-        <v>45320</v>
+        <v>45349</v>
       </c>
       <c r="C3" s="2">
-        <v>45348</v>
+        <v>45379</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2">
-        <v>45289</v>
+        <v>45320</v>
       </c>
       <c r="C4" s="2">
-        <v>45319</v>
+        <v>45348</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2">
-        <v>45258</v>
+        <v>45289</v>
       </c>
       <c r="C5" s="2">
-        <v>45288</v>
+        <v>45319</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2">
-        <v>45228</v>
+        <v>45258</v>
       </c>
       <c r="C6" s="2">
-        <v>45257</v>
+        <v>45288</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2">
-        <v>45197</v>
+        <v>45228</v>
       </c>
       <c r="C7" s="2">
-        <v>45227</v>
+        <v>45257</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2">
-        <v>45167</v>
+        <v>45197</v>
       </c>
       <c r="C8" s="2">
-        <v>45196</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2">
-        <v>45136</v>
+        <v>45167</v>
       </c>
       <c r="C9" s="2">
-        <v>45166</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2">
-        <v>45105</v>
+        <v>45136</v>
       </c>
       <c r="C10" s="2">
-        <v>45135</v>
+        <v>45166</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2">
-        <v>45075</v>
+        <v>45105</v>
       </c>
       <c r="C11" s="2">
-        <v>45104</v>
+        <v>45135</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2">
-        <v>45044</v>
+        <v>45075</v>
       </c>
       <c r="C12" s="2">
-        <v>45074</v>
+        <v>45104</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
-        <v>45014</v>
+        <v>45044</v>
       </c>
       <c r="C13" s="2">
-        <v>45043</v>
+        <v>45074</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2">
-        <v>44983</v>
+        <v>45014</v>
       </c>
       <c r="C14" s="2">
-        <v>45013</v>
+        <v>45043</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2">
-        <v>44955</v>
+        <v>44983</v>
       </c>
       <c r="C15" s="2">
-        <v>44982</v>
+        <v>45013</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
-        <v>44924</v>
+        <v>44955</v>
       </c>
       <c r="C16" s="2">
-        <v>44954</v>
+        <v>44982</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
-        <v>44893</v>
+        <v>44924</v>
       </c>
       <c r="C17" s="2">
-        <v>44923</v>
+        <v>44954</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="C18" s="2">
-        <v>44892</v>
+        <v>44923</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2">
-        <v>44832</v>
+        <v>44863</v>
       </c>
       <c r="C19" s="2">
-        <v>44862</v>
+        <v>44892</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
-        <v>44802</v>
+        <v>44832</v>
       </c>
       <c r="C20" s="2">
-        <v>44831</v>
+        <v>44862</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2">
-        <v>44771</v>
+        <v>44802</v>
       </c>
       <c r="C21" s="2">
-        <v>44801</v>
+        <v>44831</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>44740</v>
+        <v>44771</v>
       </c>
       <c r="C22" s="2">
-        <v>44770</v>
+        <v>44801</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>44710</v>
+        <v>44740</v>
       </c>
       <c r="C23" s="2">
-        <v>44739</v>
+        <v>44770</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>44679</v>
+        <v>44710</v>
       </c>
       <c r="C24" s="2">
-        <v>44709</v>
+        <v>44739</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2">
-        <v>44649</v>
+        <v>44679</v>
       </c>
       <c r="C25" s="2">
-        <v>44678</v>
+        <v>44709</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
-        <v>44618</v>
+        <v>44649</v>
       </c>
       <c r="C26" s="2">
-        <v>44648</v>
+        <v>44678</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2">
-        <v>44590</v>
+        <v>44618</v>
       </c>
       <c r="C27" s="2">
-        <v>44617</v>
+        <v>44648</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2">
-        <v>44559</v>
+        <v>44590</v>
       </c>
       <c r="C28" s="2">
-        <v>44589</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2">
-        <v>44528</v>
+        <v>44559</v>
       </c>
       <c r="C29" s="2">
-        <v>44558</v>
+        <v>44589</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2">
-        <v>44498</v>
+        <v>44528</v>
       </c>
       <c r="C30" s="2">
-        <v>44527</v>
+        <v>44558</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2">
-        <v>44467</v>
+        <v>44498</v>
       </c>
       <c r="C31" s="2">
-        <v>44497</v>
+        <v>44527</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" s="2">
-        <v>44437</v>
+        <v>44467</v>
       </c>
       <c r="C32" s="2">
-        <v>44466</v>
+        <v>44497</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2">
-        <v>44406</v>
+        <v>44437</v>
       </c>
       <c r="C33" s="2">
-        <v>44436</v>
+        <v>44466</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="2">
-        <v>44375</v>
+        <v>44406</v>
       </c>
       <c r="C34" s="2">
-        <v>44405</v>
+        <v>44436</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" s="2">
-        <v>44345</v>
+        <v>44375</v>
       </c>
       <c r="C35" s="2">
-        <v>44374</v>
+        <v>44405</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2">
-        <v>44314</v>
+        <v>44345</v>
       </c>
       <c r="C36" s="2">
-        <v>44344</v>
+        <v>44374</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" s="2">
-        <v>44284</v>
+        <v>44314</v>
       </c>
       <c r="C37" s="2">
-        <v>44313</v>
+        <v>44344</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B38" s="2">
-        <v>44253</v>
+        <v>44284</v>
       </c>
       <c r="C38" s="2">
-        <v>44283</v>
+        <v>44313</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B39" s="2">
-        <v>44225</v>
+        <v>44253</v>
       </c>
       <c r="C39" s="2">
-        <v>44252</v>
+        <v>44283</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2">
-        <v>44194</v>
+        <v>44225</v>
       </c>
       <c r="C40" s="2">
-        <v>44224</v>
+        <v>44252</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B41" s="2">
-        <v>44163</v>
+        <v>44194</v>
       </c>
       <c r="C41" s="2">
-        <v>44193</v>
+        <v>44224</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
-        <v>44133</v>
+        <v>44163</v>
       </c>
       <c r="C42" s="2">
-        <v>44162</v>
+        <v>44193</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B43" s="2">
-        <v>44102</v>
+        <v>44133</v>
       </c>
       <c r="C43" s="2">
-        <v>44132</v>
+        <v>44162</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B44" s="2">
-        <v>44072</v>
+        <v>44102</v>
       </c>
       <c r="C44" s="2">
-        <v>44101</v>
+        <v>44132</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2">
+        <v>44072</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
         <v>1</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B46" s="2">
         <v>44041</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C46" s="2">
         <v>44071</v>
       </c>
     </row>

</xml_diff>